<commit_message>
feat(mac): use new sap materials upload template (UFTABI-6999) (#5937)
* feat(mac): use new sap materials upload template

* fix(mac): fix unit tests for jenkins

* feat(mac): parse excel in new format

* feat(mac): sap materials upload validation

* fix(mac): percentage display, extended tests
fix(mac): dynamic headers

---------

Co-authored-by: konramic <konramic@schaeffler.com>
</commit_message>
<xml_diff>
--- a/apps/mac/src/assets/templates/matnr_upload_template.xlsx
+++ b/apps/mac/src/assets/templates/matnr_upload_template.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KONRAMIC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\frontend-schaeffler\apps\mac\src\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAFF373-3579-445B-9DEC-36726AB11151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A225D69-D0B7-416B-B004-865B59654EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26580" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="326" xr2:uid="{C55B1059-0EC5-41E2-AEE6-97D4155FE72A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template Version 2" sheetId="7" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -33,55 +36,241 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>plant</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>materialNumber</t>
-  </si>
-  <si>
-    <t>materialDescription</t>
-  </si>
-  <si>
-    <t>materialGroup</t>
-  </si>
-  <si>
-    <t>businessPartnerId</t>
-  </si>
-  <si>
-    <t>supplierId</t>
-  </si>
-  <si>
-    <t>supplierCountry</t>
-  </si>
-  <si>
-    <t>supplierRegion</t>
-  </si>
-  <si>
-    <t>emissionFactorKg</t>
-  </si>
-  <si>
-    <t>emissionFactorPc</t>
-  </si>
-  <si>
-    <t>dataComment</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Valid From</t>
+  </si>
+  <si>
+    <t>Valid Until</t>
+  </si>
+  <si>
+    <t>Secondary data sources</t>
+  </si>
+  <si>
+    <t>Cross Sectoral Standards Used</t>
+  </si>
+  <si>
+    <t>Customer calculation method applied</t>
+  </si>
+  <si>
+    <t>Link to customer calculation method</t>
+  </si>
+  <si>
+    <t>PCF verified by 3rd party</t>
+  </si>
+  <si>
+    <t>Net weight</t>
+  </si>
+  <si>
+    <t>Transport emissions 
+(if supplier responsibility) [kg CO2e per part]</t>
+  </si>
+  <si>
+    <t>Shipment from Supplier Location</t>
+  </si>
+  <si>
+    <t>Shipment to Schaeffler Plant</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Yes / No</t>
+  </si>
+  <si>
+    <t>DQR primary</t>
+  </si>
+  <si>
+    <t>DQR secondary</t>
+  </si>
+  <si>
+    <t>Raw material manufacturer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incoterms </t>
+  </si>
+  <si>
+    <t>DAP/FCA/FOB</t>
+  </si>
+  <si>
+    <t>Weight data source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplier | Drawing | Master data </t>
+  </si>
+  <si>
+    <t>Raw material emission factor</t>
+  </si>
+  <si>
+    <t>Material group of raw material</t>
+  </si>
+  <si>
+    <t>Fossil energy share</t>
+  </si>
+  <si>
+    <t>Link to 3rd party verification proof</t>
+  </si>
+  <si>
+    <t>Material utilization factor</t>
+  </si>
+  <si>
+    <t>Secondary material share</t>
+  </si>
+  <si>
+    <t>Recycled material share</t>
+  </si>
+  <si>
+    <t>Primary Data Share</t>
+  </si>
+  <si>
+    <t>PCF logistics</t>
+  </si>
+  <si>
+    <t>Service/Input/Gross weight</t>
+  </si>
+  <si>
+    <t>Net weight / Service weight (&lt; 1)</t>
+  </si>
+  <si>
+    <t>URI to sharepoint / etc.</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>(drawing or supplier input) [kg]</t>
+  </si>
+  <si>
+    <t>Format: 111122222 -1111-22</t>
+  </si>
+  <si>
+    <t>Material number (*)</t>
+  </si>
+  <si>
+    <t>Description (*)</t>
+  </si>
+  <si>
+    <t>Category (*)</t>
+  </si>
+  <si>
+    <t>Material Group (*)</t>
+  </si>
+  <si>
+    <t>BusinessPartnerId (*)</t>
+  </si>
+  <si>
+    <t>SupplierId (*)</t>
+  </si>
+  <si>
+    <t>PCF per kg (*)</t>
+  </si>
+  <si>
+    <t>PCF per part (*)</t>
+  </si>
+  <si>
+    <t>Product Carbon Footprint in [kg CO2e per kg] - one pcf value is mandatory</t>
+  </si>
+  <si>
+    <t>Product Carbon Footprint in [kg CO2e per part]  - one pcf value is mandatory</t>
+  </si>
+  <si>
+    <t>[%] (0.01 = 1%)</t>
+  </si>
+  <si>
+    <t>production locations [%] (0.01 = 1%)</t>
+  </si>
+  <si>
+    <t>PDS [%] (0.01 = 1%)</t>
+  </si>
+  <si>
+    <t>Supplier Country (*)</t>
+  </si>
+  <si>
+    <t>Supplier Region (*)</t>
+  </si>
+  <si>
+    <t>Iso Code</t>
+  </si>
+  <si>
+    <t>EU / AM / AP / GC</t>
+  </si>
+  <si>
+    <t>Supplier location</t>
+  </si>
+  <si>
+    <t>Plant (*)</t>
+  </si>
+  <si>
+    <t>Nuclear energy share</t>
+  </si>
+  <si>
+    <t>Renewable energy share</t>
+  </si>
+  <si>
+    <t>Only renewable electricity</t>
+  </si>
+  <si>
+    <t>(M0**-CountryCode)</t>
+  </si>
+  <si>
+    <t>(kg CO2e/kg)</t>
+  </si>
+  <si>
+    <t>Process surcharge</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Calculation method verified by 3rd party</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###,000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1F497D"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -91,22 +280,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F1"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -116,35 +305,90 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color theme="3" tint="-0.24994659260841701"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color theme="3" tint="-0.24994659260841701"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color theme="3" tint="-0.24994659260841701"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color theme="3" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="SAPMemberCell" xfId="1" xr:uid="{90757A81-E097-4DBA-ADE3-8DCB6A0F8CA3}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="2" xr:uid="{F1F020BB-086E-4865-8679-2C31060934B8}"/>
+    <cellStyle name="Standard 2 2" xfId="3" xr:uid="{84AFCB73-6E51-4686-B695-C4F99129D399}"/>
+    <cellStyle name="Text" xfId="4" xr:uid="{502EC162-D4E5-466D-9A53-BB50A5D71841}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -167,44 +411,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -254,9 +498,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -312,232 +556,436 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB3EC57-CCA6-4D6C-A5B5-51A6CF030B1F}">
+  <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.44140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.33203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="12.44140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="9.109375" style="1"/>
+    <col min="24" max="24" width="10.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="20.5546875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="20.44140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="18.44140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="20.109375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="29.88671875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15.44140625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="18.33203125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="23.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.88671875" style="1" customWidth="1"/>
+    <col min="35" max="35" width="19.33203125" style="1" customWidth="1"/>
+    <col min="36" max="36" width="12" style="1" customWidth="1"/>
+    <col min="37" max="37" width="17.6640625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="19.5546875" style="1" customWidth="1"/>
+    <col min="39" max="39" width="15" style="1" customWidth="1"/>
+    <col min="40" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:41" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="V1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="Z1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="AA1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="AB1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="AC1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" s="3" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
+      <c r="AI2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO2" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
+    <row r="3" spans="1:41" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="599" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;8&amp;K000000INTERNAL</oddFooter>
   </headerFooter>
@@ -854,21 +1302,21 @@
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <_dlc_DocId xmlns="526cfb31-bfa9-430b-8f9e-63c1bf3fd028">OG37413-1167607063-1907</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="526cfb31-bfa9-430b-8f9e-63c1bf3fd028">
-      <Url>https://worksite.sharepoint.com/sites/OG_37413/_layouts/15/DocIdRedir.aspx?ID=OG37413-1167607063-1907</Url>
-      <Description>OG37413-1167607063-1907</Description>
-    </_dlc_DocIdUrl>
-    <TaxCatchAll xmlns="526cfb31-bfa9-430b-8f9e-63c1bf3fd028" xsi:nil="true"/>
+    <_dlc_DocId xmlns="526cfb31-bfa9-430b-8f9e-63c1bf3fd028">OG37413-1167607063-1956</_dlc_DocId>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="828b9f9e-0483-4910-8f4f-7397cd9a01b8">
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="526cfb31-bfa9-430b-8f9e-63c1bf3fd028" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="526cfb31-bfa9-430b-8f9e-63c1bf3fd028">
+      <Url>https://worksite.sharepoint.com/sites/OG_37413/_layouts/15/DocIdRedir.aspx?ID=OG37413-1167607063-1956</Url>
+      <Description>OG37413-1167607063-1956</Description>
+    </_dlc_DocIdUrl>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80D3DF9F-32F5-497E-BF60-50D993372C43}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C34FAAF7-564D-4627-865F-AC6F7E58A59A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -887,7 +1335,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F282DC94-0706-4C8C-BB78-3540DB8FC801}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CDA5F52-4056-451E-9AC7-74D660B8B193}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
@@ -895,7 +1343,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53D7BC34-2451-4C85-83D5-71659017ED9F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8280762D-179B-4E40-B452-CFDE0EAEFD47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
@@ -903,7 +1351,7 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73FD8F81-4158-4A64-8040-2D2DD9B39725}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276CAC86-CFD9-4DF2-AD3E-26CDEFED06A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>

</xml_diff>